<commit_message>
DCC_UI_blank.xlsx was made blank of content except for the exsitence of 	the sheet named 'definitions'.
</commit_message>
<xml_diff>
--- a/DCC_UI_blank.xlsx
+++ b/DCC_UI_blank.xlsx
@@ -8,17 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tesla\data\MS\DBH\Projects\1901 NY-INFRA-FOT\DCC\Software\DCCtables\master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259A820E-249F-4A37-8D65-076AFABD4C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85B6A31-A116-417F-859D-7523580CB3E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="37220" windowHeight="21820" tabRatio="788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7730" yWindow="3980" windowWidth="24470" windowHeight="15220" tabRatio="788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="2" r:id="rId1"/>
-    <sheet name="Software" sheetId="8" state="hidden" r:id="rId2"/>
-    <sheet name="Locations" sheetId="15" state="hidden" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
+    <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
     <definedName name="accreditationApplicabilityType">Definitions!$E$2:$E$3</definedName>
@@ -73,189 +71,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>DFM A/S</t>
-  </si>
-  <si>
-    <t>Administration@dfm.dk</t>
-  </si>
-  <si>
-    <t>+45 7730 5800</t>
-  </si>
-  <si>
-    <t>Hørsholm</t>
-  </si>
-  <si>
-    <t>DK</t>
-  </si>
-  <si>
-    <t>2970</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>www.dfm.dk</t>
-  </si>
-  <si>
-    <t>Danish Measurement Company Ltd.</t>
-  </si>
-  <si>
-    <t>mm@dmc.dk</t>
-  </si>
-  <si>
-    <t>Måløv</t>
-  </si>
-  <si>
-    <t>9899</t>
-  </si>
-  <si>
-    <t>Målervej</t>
-  </si>
-  <si>
-    <t>16, 1. sal</t>
-  </si>
-  <si>
-    <t>Mads Målermand</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>swID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">release </t>
-  </si>
-  <si>
-    <t>type</t>
-  </si>
-  <si>
-    <t>content</t>
-  </si>
-  <si>
-    <t>file</t>
-  </si>
-  <si>
-    <t>formula</t>
-  </si>
-  <si>
-    <t>Kogle Alle</t>
-  </si>
-  <si>
-    <t>laboratory</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>City</t>
-  </si>
-  <si>
-    <t>cust</t>
-  </si>
-  <si>
-    <t>lab</t>
-  </si>
-  <si>
-    <t>Street1</t>
-  </si>
-  <si>
-    <t>heading lang1</t>
-  </si>
-  <si>
-    <t>heading lang2</t>
-  </si>
-  <si>
-    <t>34507624</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>CompanyName</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>PostalCode</t>
-  </si>
-  <si>
-    <t>Street_No</t>
-  </si>
-  <si>
-    <t>Webpage</t>
-  </si>
-  <si>
-    <t>Street2</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Att</t>
-  </si>
-  <si>
-    <t>Company name</t>
-  </si>
-  <si>
-    <t>Firmanavn</t>
-  </si>
-  <si>
-    <t>Tel.:</t>
-  </si>
-  <si>
-    <t>email:</t>
-  </si>
-  <si>
-    <t>Phone:</t>
-  </si>
-  <si>
-    <t>City:</t>
-  </si>
-  <si>
-    <t>By:</t>
-  </si>
-  <si>
-    <t>Landekode:</t>
-  </si>
-  <si>
-    <t>Country code</t>
-  </si>
-  <si>
-    <t>Postal Code</t>
-  </si>
-  <si>
-    <t>Postnr.:</t>
-  </si>
-  <si>
-    <t>Calibration laboratory</t>
-  </si>
-  <si>
-    <t>Kalibreringslaboratoriet</t>
-  </si>
-  <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t>Kunde</t>
   </si>
   <si>
     <t>Parameter</t>
@@ -277,7 +95,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,14 +122,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -330,44 +140,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -530,23 +317,6 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table14" displayName="Table14" ref="A1:H6" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:H6" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="swID"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="name"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="release "/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="type"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="description"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="content"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="file"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="formula"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -871,7 +641,7 @@
   <sheetData>
     <row r="1" spans="1:12" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
-        <v>61</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -879,19 +649,19 @@
     </row>
     <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>65</v>
+        <v>5</v>
       </c>
       <c r="L2" s="1"/>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>63</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="L3" s="1"/>
     </row>
@@ -940,297 +710,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:I1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P46" sqref="P46"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.81640625" customWidth="1"/>
-    <col min="8" max="8" width="9.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:P16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
-    <col min="2" max="2" width="25.54296875" customWidth="1"/>
-    <col min="3" max="3" width="34.81640625" customWidth="1"/>
-    <col min="4" max="4" width="16.453125" customWidth="1"/>
-    <col min="5" max="5" width="15.453125" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" customWidth="1"/>
-    <col min="12" max="12" width="13.81640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="B1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G1" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J1" t="s">
-        <v>27</v>
-      </c>
-      <c r="K1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
-        <v>39</v>
-      </c>
-      <c r="M1" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I2" t="s">
-        <v>50</v>
-      </c>
-      <c r="J2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" t="s">
-        <v>54</v>
-      </c>
-      <c r="L2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" t="s">
-        <v>53</v>
-      </c>
-      <c r="L3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" t="s">
-        <v>5</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="B9" s="3"/>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="B15" s="5"/>
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="B16" s="4"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="O4" r:id="rId1" display="www.dfm.dk" xr:uid="{D844B87A-F6B8-451D-B8BF-975CF3E92642}"/>
-    <hyperlink ref="H4" r:id="rId2" xr:uid="{73FD074B-6D0C-4999-ACA1-30AD886FD9AB}"/>
-    <hyperlink ref="P4" r:id="rId3" xr:uid="{153A4F9C-AACC-4026-9BDC-B9B73A9C4501}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{0AF9D9D2-0BDE-4EE4-8AF5-708EE8F6F186}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>